<commit_message>
Add database population tests
</commit_message>
<xml_diff>
--- a/services/django/app/src/data/excel_files/exam_timetable_for_invigilation.xlsx
+++ b/services/django/app/src/data/excel_files/exam_timetable_for_invigilation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pipsk\Documents\uni\ComputerScience\Year3\PSD\Project\jh03-main\services\django\app\src\data\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C13EA2A-DE63-45C8-A0F2-C5BA077EE6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9242340A-6EBE-4499-907B-60DF4F1AE07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9FCE311A-559C-4362-BED6-824406A09276}"/>
   </bookViews>
@@ -4934,7 +4934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F89E1EE-2CF9-4D7F-828D-9CD0C94F3791}">
   <dimension ref="A1:S649"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>